<commit_message>
find ./db.conf & update-dw 20180615
</commit_message>
<xml_diff>
--- a/test-temp2.xlsx
+++ b/test-temp2.xlsx
@@ -9,27 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>third</t>
-  </si>
-  <si>
-    <t>first</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>second</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -361,31 +354,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1">
+        <v>44</v>
+      </c>
+      <c r="B1">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>34</v>
+      </c>
+      <c r="B2" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B11">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="n">
-        <v>11.0</v>
+        <v>31.0</v>
       </c>
       <c r="B1" t="n">
-        <v>12.0</v>
+        <v>32.0</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B11">
-        <v>99</v>
+      <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev002 .sql take args 20180629
</commit_message>
<xml_diff>
--- a/test-temp2.xlsx
+++ b/test-temp2.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet3" r:id="rId3" sheetId="1"/>
-    <sheet name="sheet4" r:id="rId4" sheetId="2"/>
+    <sheet name="sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="sheet2" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>